<commit_message>
completed generation of clade structure JSONs from Kiki's spreadsheet.
</commit_message>
<xml_diff>
--- a/tabular/contributed/REFERENCE GENOMES_for_Josh.xlsx
+++ b/tabular/contributed/REFERENCE GENOMES_for_Josh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="5920" windowWidth="39740" windowHeight="23020"/>
+    <workbookView xWindow="9000" yWindow="2620" windowWidth="39740" windowHeight="23020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="1082">
   <si>
     <t>JX272539</t>
   </si>
@@ -3006,9 +3006,6 @@
   </si>
   <si>
     <t>KY365755</t>
-  </si>
-  <si>
-    <t>BTV-LIKE</t>
   </si>
   <si>
     <t>KF563945</t>
@@ -3796,9 +3793,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y788"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U68" sqref="U68"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P69" sqref="P69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3893,7 +3890,7 @@
         <v>914</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>91</v>
@@ -3949,7 +3946,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>921</v>
@@ -4005,7 +4002,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>921</v>
@@ -4059,7 +4056,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>922</v>
@@ -4113,7 +4110,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>922</v>
@@ -4167,7 +4164,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>922</v>
@@ -4221,7 +4218,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>922</v>
@@ -4275,7 +4272,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>922</v>
@@ -4329,7 +4326,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>922</v>
@@ -4356,7 +4353,7 @@
         <v>755</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="P10" s="4">
         <v>9</v>
@@ -4412,7 +4409,7 @@
         <v>986</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="P11" s="4">
         <v>10</v>
@@ -4466,7 +4463,7 @@
         <v>756</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="P12" s="4">
         <v>11</v>
@@ -4520,7 +4517,7 @@
         <v>757</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="P13" s="4">
         <v>12</v>
@@ -4574,7 +4571,7 @@
         <v>758</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="P14" s="4">
         <v>13</v>
@@ -4659,7 +4656,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>919</v>
@@ -4900,7 +4897,7 @@
         <v>811</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="P20" s="4">
         <v>19</v>
@@ -4954,7 +4951,7 @@
         <v>812</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="P21" s="4">
         <v>20</v>
@@ -5008,7 +5005,7 @@
         <v>813</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="P22" s="4">
         <v>21</v>
@@ -5062,7 +5059,7 @@
         <v>814</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="P23" s="4">
         <v>22</v>
@@ -5333,7 +5330,7 @@
         <v>8</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="O28" s="4">
         <v>7</v>
@@ -6112,7 +6109,7 @@
         <v>4</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="V42" s="11" t="s">
         <v>922</v>
@@ -6318,7 +6315,7 @@
         <v>807</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="P46" s="4">
         <v>45</v>
@@ -6372,7 +6369,7 @@
         <v>808</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="P47" s="4">
         <v>46</v>
@@ -6426,7 +6423,7 @@
         <v>809</v>
       </c>
       <c r="O48" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="P48" s="4">
         <v>47</v>
@@ -6480,7 +6477,7 @@
         <v>810</v>
       </c>
       <c r="O49" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="P49" s="4">
         <v>48</v>
@@ -7080,7 +7077,7 @@
         <v>868</v>
       </c>
       <c r="O60" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P60" s="4">
         <v>59</v>
@@ -7134,7 +7131,7 @@
         <v>869</v>
       </c>
       <c r="O61" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P61" s="4">
         <v>60</v>
@@ -7188,7 +7185,7 @@
         <v>870</v>
       </c>
       <c r="O62" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P62" s="4">
         <v>61</v>
@@ -7242,7 +7239,7 @@
         <v>871</v>
       </c>
       <c r="O63" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P63" s="4">
         <v>62</v>
@@ -7296,7 +7293,7 @@
         <v>872</v>
       </c>
       <c r="O64" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P64" s="4">
         <v>63</v>
@@ -7350,7 +7347,7 @@
         <v>873</v>
       </c>
       <c r="O65" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P65" s="4">
         <v>64</v>
@@ -7404,7 +7401,7 @@
         <v>874</v>
       </c>
       <c r="O66" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P66" s="4">
         <v>65</v>
@@ -7457,8 +7454,8 @@
       <c r="N67" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="O67" s="4" t="s">
-        <v>990</v>
+      <c r="O67" s="4">
+        <v>27</v>
       </c>
       <c r="P67" s="4">
         <v>66</v>
@@ -7511,8 +7508,8 @@
       <c r="N68" s="1" t="s">
         <v>989</v>
       </c>
-      <c r="O68" s="4" t="s">
-        <v>990</v>
+      <c r="O68" s="4">
+        <v>27</v>
       </c>
       <c r="P68" s="4">
         <v>67</v>
@@ -7524,7 +7521,7 @@
         <v>5</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="V68" s="11" t="s">
         <v>91</v>
@@ -7565,8 +7562,8 @@
       <c r="N69" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="O69" s="4" t="s">
-        <v>990</v>
+      <c r="O69" s="4">
+        <v>27</v>
       </c>
       <c r="P69" s="4">
         <v>68</v>
@@ -7890,7 +7887,7 @@
         <v>773</v>
       </c>
       <c r="O75" s="4" t="s">
-        <v>990</v>
+        <v>1066</v>
       </c>
       <c r="P75" s="4">
         <v>74</v>
@@ -7944,7 +7941,7 @@
         <v>774</v>
       </c>
       <c r="O76" s="4" t="s">
-        <v>990</v>
+        <v>1066</v>
       </c>
       <c r="P76" s="4">
         <v>75</v>
@@ -8056,7 +8053,7 @@
         <v>819</v>
       </c>
       <c r="O78" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P78" s="4">
         <v>77</v>
@@ -8110,7 +8107,7 @@
         <v>820</v>
       </c>
       <c r="O79" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P79" s="4">
         <v>78</v>
@@ -8164,7 +8161,7 @@
         <v>821</v>
       </c>
       <c r="O80" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P80" s="4">
         <v>79</v>
@@ -8218,7 +8215,7 @@
         <v>822</v>
       </c>
       <c r="O81" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P81" s="4">
         <v>80</v>
@@ -8272,7 +8269,7 @@
         <v>823</v>
       </c>
       <c r="O82" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P82" s="4">
         <v>81</v>
@@ -8323,10 +8320,10 @@
         <v>19</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="O83" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P83" s="4">
         <v>82</v>
@@ -8380,7 +8377,7 @@
         <v>824</v>
       </c>
       <c r="O84" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P84" s="4">
         <v>83</v>
@@ -8434,7 +8431,7 @@
         <v>825</v>
       </c>
       <c r="O85" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P85" s="4">
         <v>84</v>
@@ -8488,7 +8485,7 @@
         <v>826</v>
       </c>
       <c r="O86" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P86" s="4">
         <v>85</v>
@@ -8542,7 +8539,7 @@
         <v>827</v>
       </c>
       <c r="O87" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P87" s="4">
         <v>86</v>
@@ -8596,7 +8593,7 @@
         <v>828</v>
       </c>
       <c r="O88" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P88" s="4">
         <v>87</v>
@@ -8650,7 +8647,7 @@
         <v>829</v>
       </c>
       <c r="O89" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P89" s="4">
         <v>88</v>
@@ -8704,7 +8701,7 @@
         <v>830</v>
       </c>
       <c r="O90" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P90" s="4">
         <v>89</v>
@@ -8758,7 +8755,7 @@
         <v>831</v>
       </c>
       <c r="O91" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P91" s="4">
         <v>90</v>
@@ -8812,7 +8809,7 @@
         <v>832</v>
       </c>
       <c r="O92" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P92" s="4">
         <v>91</v>
@@ -8841,7 +8838,7 @@
         <v>914</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D93" s="11" t="s">
         <v>91</v>
@@ -8866,7 +8863,7 @@
         <v>833</v>
       </c>
       <c r="O93" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P93" s="4">
         <v>92</v>
@@ -8895,7 +8892,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D94" s="11" t="s">
         <v>921</v>
@@ -8920,7 +8917,7 @@
         <v>834</v>
       </c>
       <c r="O94" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P94" s="4">
         <v>93</v>
@@ -8949,7 +8946,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D95" s="11" t="s">
         <v>921</v>
@@ -8976,7 +8973,7 @@
         <v>835</v>
       </c>
       <c r="O95" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="P95" s="4">
         <v>94</v>
@@ -9005,7 +9002,7 @@
         <v>2</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D96" s="11" t="s">
         <v>922</v>
@@ -9030,7 +9027,7 @@
         <v>836</v>
       </c>
       <c r="O96" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="P96" s="4">
         <v>95</v>
@@ -9059,7 +9056,7 @@
         <v>2</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D97" s="11" t="s">
         <v>922</v>
@@ -9084,7 +9081,7 @@
         <v>837</v>
       </c>
       <c r="O97" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="P97" s="4">
         <v>96</v>
@@ -9113,7 +9110,7 @@
         <v>2</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D98" s="11" t="s">
         <v>922</v>
@@ -9138,7 +9135,7 @@
         <v>838</v>
       </c>
       <c r="O98" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P98" s="4">
         <v>97</v>
@@ -9167,7 +9164,7 @@
         <v>2</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D99" s="11" t="s">
         <v>922</v>
@@ -9192,7 +9189,7 @@
         <v>839</v>
       </c>
       <c r="O99" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P99" s="4">
         <v>98</v>
@@ -9221,7 +9218,7 @@
         <v>2</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D100" s="11" t="s">
         <v>922</v>
@@ -9246,7 +9243,7 @@
         <v>840</v>
       </c>
       <c r="O100" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P100" s="4">
         <v>99</v>
@@ -9275,7 +9272,7 @@
         <v>2</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D101" s="11" t="s">
         <v>922</v>
@@ -9300,7 +9297,7 @@
         <v>841</v>
       </c>
       <c r="O101" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P101" s="4">
         <v>100</v>
@@ -9354,7 +9351,7 @@
         <v>842</v>
       </c>
       <c r="O102" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P102" s="4">
         <v>101</v>
@@ -9408,7 +9405,7 @@
         <v>843</v>
       </c>
       <c r="O103" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P103" s="4">
         <v>102</v>
@@ -9462,7 +9459,7 @@
         <v>844</v>
       </c>
       <c r="O104" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P104" s="4">
         <v>103</v>
@@ -9516,7 +9513,7 @@
         <v>845</v>
       </c>
       <c r="O105" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P105" s="4">
         <v>104</v>
@@ -10007,7 +10004,7 @@
         <v>25</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="O114" s="4">
         <v>14</v>
@@ -10274,7 +10271,7 @@
         <v>875</v>
       </c>
       <c r="O120" s="4" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="P120" s="4">
         <v>119</v>
@@ -10313,7 +10310,7 @@
         <v>876</v>
       </c>
       <c r="O121" s="4" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="P121" s="4">
         <v>120</v>
@@ -10352,7 +10349,7 @@
         <v>877</v>
       </c>
       <c r="O122" s="4" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="P122" s="4">
         <v>121</v>
@@ -10393,7 +10390,7 @@
         <v>776</v>
       </c>
       <c r="O123" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P123" s="4">
         <v>122</v>
@@ -10432,7 +10429,7 @@
         <v>777</v>
       </c>
       <c r="O124" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P124" s="4">
         <v>123</v>
@@ -10471,7 +10468,7 @@
         <v>778</v>
       </c>
       <c r="O125" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P125" s="4">
         <v>124</v>
@@ -10510,7 +10507,7 @@
         <v>779</v>
       </c>
       <c r="O126" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P126" s="4">
         <v>125</v>
@@ -10549,7 +10546,7 @@
         <v>780</v>
       </c>
       <c r="O127" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P127" s="4">
         <v>126</v>
@@ -10588,7 +10585,7 @@
         <v>781</v>
       </c>
       <c r="O128" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P128" s="4">
         <v>127</v>
@@ -10627,7 +10624,7 @@
         <v>782</v>
       </c>
       <c r="O129" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P129" s="4">
         <v>128</v>
@@ -10666,7 +10663,7 @@
         <v>783</v>
       </c>
       <c r="O130" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P130" s="4">
         <v>129</v>
@@ -10705,7 +10702,7 @@
         <v>784</v>
       </c>
       <c r="O131" s="4" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="P131" s="4">
         <v>130</v>
@@ -10744,7 +10741,7 @@
         <v>785</v>
       </c>
       <c r="O132" s="4" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="P132" s="4">
         <v>131</v>
@@ -10982,7 +10979,7 @@
         <v>883</v>
       </c>
       <c r="O138" s="4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="P138" s="4">
         <v>137</v>
@@ -11021,7 +11018,7 @@
         <v>884</v>
       </c>
       <c r="O139" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P139" s="4">
         <v>138</v>
@@ -11060,7 +11057,7 @@
         <v>885</v>
       </c>
       <c r="O140" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P140" s="4">
         <v>139</v>
@@ -11099,7 +11096,7 @@
         <v>886</v>
       </c>
       <c r="O141" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P141" s="4">
         <v>140</v>
@@ -11138,7 +11135,7 @@
         <v>887</v>
       </c>
       <c r="O142" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P142" s="4">
         <v>141</v>
@@ -11177,7 +11174,7 @@
         <v>888</v>
       </c>
       <c r="O143" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P143" s="4">
         <v>142</v>
@@ -11216,7 +11213,7 @@
         <v>889</v>
       </c>
       <c r="O144" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P144" s="4">
         <v>143</v>
@@ -11255,7 +11252,7 @@
         <v>890</v>
       </c>
       <c r="O145" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P145" s="4">
         <v>144</v>
@@ -11294,7 +11291,7 @@
         <v>891</v>
       </c>
       <c r="O146" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P146" s="4">
         <v>145</v>
@@ -11939,7 +11936,7 @@
         <v>1</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D184" s="11" t="s">
         <v>921</v>
@@ -11956,7 +11953,7 @@
         <v>1</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D185" s="11" t="s">
         <v>921</v>
@@ -11973,7 +11970,7 @@
         <v>1</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D186" s="11" t="s">
         <v>921</v>
@@ -11990,7 +11987,7 @@
         <v>2</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D187" s="11" t="s">
         <v>922</v>
@@ -12007,7 +12004,7 @@
         <v>2</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D188" s="11" t="s">
         <v>922</v>
@@ -12024,7 +12021,7 @@
         <v>2</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D189" s="11" t="s">
         <v>922</v>
@@ -12075,7 +12072,7 @@
         <v>3</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D192" s="11" t="s">
         <v>931</v>
@@ -12092,7 +12089,7 @@
         <v>3</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D193" s="11" t="s">
         <v>931</v>
@@ -13486,7 +13483,7 @@
         <v>1</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D275" s="11" t="s">
         <v>91</v>
@@ -13503,7 +13500,7 @@
         <v>1</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D276" s="11" t="s">
         <v>91</v>
@@ -13520,7 +13517,7 @@
         <v>2</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D277" s="11" t="s">
         <v>922</v>
@@ -13537,7 +13534,7 @@
         <v>2</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D278" s="11" t="s">
         <v>922</v>
@@ -13554,7 +13551,7 @@
         <v>2</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D279" s="11" t="s">
         <v>922</v>
@@ -13571,7 +13568,7 @@
         <v>2</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D280" s="11" t="s">
         <v>922</v>
@@ -13588,7 +13585,7 @@
         <v>914</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D281" s="11" t="s">
         <v>930</v>
@@ -13605,7 +13602,7 @@
         <v>914</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D282" s="11" t="s">
         <v>931</v>
@@ -13622,7 +13619,7 @@
         <v>914</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D283" s="11" t="s">
         <v>946</v>
@@ -15924,7 +15921,7 @@
         <v>5</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D409" s="11" t="s">
         <v>950</v>
@@ -15945,7 +15942,7 @@
         <v>5</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D410" s="11" t="s">
         <v>950</v>
@@ -15966,7 +15963,7 @@
         <v>5</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D411" s="11" t="s">
         <v>950</v>
@@ -15987,7 +15984,7 @@
         <v>5</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D412" s="11" t="s">
         <v>950</v>
@@ -16008,7 +16005,7 @@
         <v>5</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D413" s="11" t="s">
         <v>950</v>
@@ -16029,7 +16026,7 @@
         <v>5</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D414" s="11" t="s">
         <v>950</v>
@@ -16050,7 +16047,7 @@
         <v>6</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D415" s="11" t="s">
         <v>951</v>
@@ -16071,7 +16068,7 @@
         <v>6</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D416" s="11" t="s">
         <v>951</v>
@@ -17142,7 +17139,7 @@
         <v>932</v>
       </c>
       <c r="C467" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D467" s="11" t="s">
         <v>91</v>
@@ -17159,7 +17156,7 @@
         <v>1</v>
       </c>
       <c r="C468" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D468" s="11" t="s">
         <v>921</v>
@@ -17176,7 +17173,7 @@
         <v>1</v>
       </c>
       <c r="C469" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D469" s="11" t="s">
         <v>921</v>
@@ -17210,7 +17207,7 @@
         <v>2</v>
       </c>
       <c r="C471" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D471" s="11" t="s">
         <v>922</v>
@@ -17227,7 +17224,7 @@
         <v>2</v>
       </c>
       <c r="C472" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D472" s="11" t="s">
         <v>922</v>
@@ -17244,7 +17241,7 @@
         <v>2</v>
       </c>
       <c r="C473" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D473" s="11" t="s">
         <v>922</v>
@@ -17261,7 +17258,7 @@
         <v>2</v>
       </c>
       <c r="C474" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D474" s="11" t="s">
         <v>922</v>
@@ -17278,7 +17275,7 @@
         <v>2</v>
       </c>
       <c r="C475" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D475" s="11" t="s">
         <v>922</v>
@@ -17924,7 +17921,7 @@
         <v>3</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D513" s="11" t="s">
         <v>919</v>
@@ -18689,7 +18686,7 @@
         <v>1</v>
       </c>
       <c r="C558" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D558" s="11" t="s">
         <v>921</v>
@@ -18706,7 +18703,7 @@
         <v>1</v>
       </c>
       <c r="C559" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D559" s="11" t="s">
         <v>921</v>
@@ -18723,7 +18720,7 @@
         <v>2</v>
       </c>
       <c r="C560" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D560" s="11" t="s">
         <v>91</v>
@@ -18740,7 +18737,7 @@
         <v>2</v>
       </c>
       <c r="C561" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D561" s="11" t="s">
         <v>91</v>
@@ -18757,7 +18754,7 @@
         <v>2</v>
       </c>
       <c r="C562" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D562" s="11" t="s">
         <v>91</v>
@@ -18774,7 +18771,7 @@
         <v>3</v>
       </c>
       <c r="C563" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D563" s="11" t="s">
         <v>922</v>
@@ -18808,7 +18805,7 @@
         <v>914</v>
       </c>
       <c r="C565" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D565" s="11" t="s">
         <v>930</v>
@@ -18825,7 +18822,7 @@
         <v>914</v>
       </c>
       <c r="C566" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D566" s="11" t="s">
         <v>931</v>
@@ -18842,7 +18839,7 @@
         <v>914</v>
       </c>
       <c r="C567" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D567" s="11" t="s">
         <v>946</v>
@@ -19046,7 +19043,7 @@
         <v>4</v>
       </c>
       <c r="C579" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D579" s="11" t="s">
         <v>920</v>
@@ -20457,7 +20454,7 @@
         <v>1</v>
       </c>
       <c r="C662" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D662" s="4" t="s">
         <v>922</v>
@@ -20478,7 +20475,7 @@
         <v>1</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D663" s="4" t="s">
         <v>922</v>
@@ -20499,7 +20496,7 @@
         <v>2</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D664" s="4" t="s">
         <v>91</v>
@@ -20520,7 +20517,7 @@
         <v>2</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D665" s="4" t="s">
         <v>91</v>
@@ -20541,7 +20538,7 @@
         <v>2</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D666" s="4" t="s">
         <v>91</v>
@@ -20562,7 +20559,7 @@
         <v>2</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D667" s="4" t="s">
         <v>91</v>
@@ -20583,7 +20580,7 @@
         <v>2</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D668" s="4" t="s">
         <v>91</v>
@@ -20604,7 +20601,7 @@
         <v>2</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D669" s="4" t="s">
         <v>91</v>
@@ -20625,7 +20622,7 @@
         <v>914</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D670" s="4" t="s">
         <v>930</v>

</xml_diff>